<commit_message>
New branch for trying Jekyll setup
</commit_message>
<xml_diff>
--- a/files/milpa-netzwerk.xlsx
+++ b/files/milpa-netzwerk.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis0\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis0\source\milpa-netzwerk-prototyp\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017F8DF2-356A-480E-8289-E6F8E64F5D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6C4360-09A3-4A27-A401-78F1F6A2BE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{27B4222C-7179-4D38-A482-7079C6DDB59D}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Allerweltshaus</t>
   </si>
@@ -74,6 +74,27 @@
   </si>
   <si>
     <t>Nominatim Wichtigkeit</t>
+  </si>
+  <si>
+    <t>Webseite</t>
+  </si>
+  <si>
+    <t>https://www.allerweltshaus.de/</t>
+  </si>
+  <si>
+    <t>https://solawi-alfter.de/</t>
+  </si>
+  <si>
+    <t>https://alsenstrasse.com/der-alsengarten/</t>
+  </si>
+  <si>
+    <t>https://urbane-gaerten.de/urbane-gaerten/gaerten-im-ueberblick/demogarten,-k%C3%B6ln</t>
+  </si>
+  <si>
+    <t>https://www.urbanes-gaertnern-freiburg.de/de/organisations/fridas-klima-garten</t>
+  </si>
+  <si>
+    <t>https://www.weltacker-berlin.de/</t>
   </si>
 </sst>
 </file>
@@ -935,22 +956,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5CD6C1-6601-4B49-A6B3-53F091B5D624}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.77734375" customWidth="1"/>
-    <col min="2" max="2" width="49.5546875" customWidth="1"/>
-    <col min="3" max="4" width="25.77734375" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" customWidth="1"/>
+    <col min="2" max="3" width="49.5546875" customWidth="1"/>
+    <col min="4" max="5" width="25.77734375" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" customWidth="1"/>
+    <col min="7" max="7" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -958,64 +979,85 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>